<commit_message>
Added Test Info Order Tests API
</commit_message>
<xml_diff>
--- a/BloodstreamAPI/testData/testinfo.xlsx
+++ b/BloodstreamAPI/testData/testinfo.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8903CC4-65C3-49AC-97C8-6D465C6509F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9F19DB30-1BD6-4546-9DA6-3F11DA6ECE92}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="2420" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12330" windowHeight="9585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GetgridLayout" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="orderTests" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:I25"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="13">
   <si>
     <t>GroupStatus</t>
   </si>
@@ -41,42 +42,9 @@
     <t>EndPoint</t>
   </si>
   <si>
-    <t>DonationCount</t>
-  </si>
-  <si>
-    <t>TestCaseName</t>
-  </si>
-  <si>
-    <t>/donationInfo/donations</t>
-  </si>
-  <si>
-    <t>DonationCount1</t>
-  </si>
-  <si>
     <t>/testInfo/orderTests</t>
   </si>
   <si>
-    <t>DonationID</t>
-  </si>
-  <si>
-    <t>Flagname</t>
-  </si>
-  <si>
-    <t>sort</t>
-  </si>
-  <si>
-    <t>PKS22PPKSDAW12341</t>
-  </si>
-  <si>
-    <t>S - Skipped error</t>
-  </si>
-  <si>
-    <t>TestGet200</t>
-  </si>
-  <si>
-    <t>TestGet401</t>
-  </si>
-  <si>
     <t>Assert200</t>
   </si>
   <si>
@@ -84,13 +52,22 @@
   </si>
   <si>
     <t>Assert401</t>
+  </si>
+  <si>
+    <t>/gridLayout/columnPreference</t>
+  </si>
+  <si>
+    <t>gridName</t>
+  </si>
+  <si>
+    <t>TestInformation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +81,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF505050"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -140,12 +123,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -160,6 +140,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -443,251 +427,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC16E1A-EBE8-4FD7-9522-847FD03243A9}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.26953125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="26.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="3" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5"/>
+    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
+    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="3" t="s">
-        <v>10</v>
-      </c>
+    <row r="12" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A18:E18"/>
+  <mergeCells count="3">
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A9:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -696,51 +593,151 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDA324F4-6303-45A9-B72B-667907D5EA0F}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="2" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A9:E9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Pool Details API
</commit_message>
<xml_diff>
--- a/BloodstreamAPI/testData/testinfo.xlsx
+++ b/BloodstreamAPI/testData/testinfo.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9F19DB30-1BD6-4546-9DA6-3F11DA6ECE92}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6EE8B454-C35B-42AC-9ACA-8E952603A7B1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12330" windowHeight="9585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12330" windowHeight="9585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GetgridLayout" sheetId="2" r:id="rId1"/>
     <sheet name="orderTests" sheetId="3" r:id="rId2"/>
+    <sheet name="poolDetails" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I25"/>
+  <oleSize ref="A1:H23"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="15">
   <si>
     <t>GroupStatus</t>
   </si>
@@ -61,6 +62,12 @@
   </si>
   <si>
     <t>TestInformation</t>
+  </si>
+  <si>
+    <t>/testInfo/poolDetail</t>
+  </si>
+  <si>
+    <t>PoolID</t>
   </si>
 </sst>
 </file>
@@ -137,13 +144,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -429,7 +436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC16E1A-EBE8-4FD7-9522-847FD03243A9}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -444,16 +451,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -488,13 +495,13 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -532,13 +539,13 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -578,7 +585,7 @@
     <row r="19" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
+      <c r="A23" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -595,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDA324F4-6303-45A9-B72B-667907D5EA0F}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,13 +615,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -652,13 +659,13 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -696,13 +703,13 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -730,6 +737,154 @@
       <c r="D11" s="4"/>
       <c r="E11" s="2" t="s">
         <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A9:E9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BEF42D-A3E4-4A88-9791-CF6A0267BCC5}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
groupstatus count for test info api added
</commit_message>
<xml_diff>
--- a/BloodstreamAPI/testData/testinfo.xlsx
+++ b/BloodstreamAPI/testData/testinfo.xlsx
@@ -3,18 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A8C07C85-F755-4CA2-ADF0-6A3ACDA90348}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0756B844-04C6-43DC-B035-B764BBB1A125}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12330" windowHeight="9585" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12330" windowHeight="9585" tabRatio="715" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GetgridLayout" sheetId="2" r:id="rId1"/>
     <sheet name="orderTests" sheetId="3" r:id="rId2"/>
     <sheet name="poolDetails" sheetId="4" r:id="rId3"/>
     <sheet name="poolConstituents" sheetId="5" r:id="rId4"/>
+    <sheet name="groupStatusCount" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L29"/>
+  <oleSize ref="A1:K29"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="17">
   <si>
     <t>GroupStatus</t>
   </si>
@@ -72,6 +73,9 @@
   </si>
   <si>
     <t>/testInfo/poolConstituents</t>
+  </si>
+  <si>
+    <t>/testInfo/groupStatusCount</t>
   </si>
 </sst>
 </file>
@@ -134,7 +138,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -155,6 +159,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -905,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3647A310-75FB-45FE-A804-D8642A60FA0E}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,4 +1054,154 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD6AE23C-ED38-43E1-8869-59A543319E62}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A9:E9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>